<commit_message>
Removed alt init system. Added medal system. More tweaks to sets.
</commit_message>
<xml_diff>
--- a/SupersNew/characters/Beetle.xlsx
+++ b/SupersNew/characters/Beetle.xlsx
@@ -372,9 +372,6 @@
     <t>Day Job: Jock</t>
   </si>
   <si>
-    <t>Tough – You start the game with +4 Hit Points.</t>
-  </si>
-  <si>
     <t>Clinging</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>Cling</t>
+  </si>
+  <si>
+    <t>Tough – You start the game with +6 Hit Points.</t>
   </si>
 </sst>
 </file>
@@ -509,6 +509,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,22 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,13 +957,13 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
@@ -974,13 +974,13 @@
       <c r="A2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="10" t="s">
         <v>27</v>
       </c>
@@ -991,13 +991,13 @@
       <c r="A3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1214,17 +1214,17 @@
         <v>74</v>
       </c>
       <c r="B15" s="4">
-        <f>_xlfn.CEILING.MATH(8+B10+B7*(0.5)+B12*(0.5) + 4)</f>
-        <v>41</v>
+        <f>_xlfn.CEILING.MATH(8+B10+B7*(0.5)+B12*(0.5) + 6)</f>
+        <v>43</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="9" t="s">
         <v>79</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1266,7 +1266,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="12"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1311,224 +1311,219 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="12">
         <v>30</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="12">
         <v>0</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="12">
         <v>20</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="12">
         <v>20</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="12">
         <v>10</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="12">
         <v>4</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="22">
         <v>20</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="22">
         <v>0</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="18" t="s">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="12">
         <v>20</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="12">
         <v>3</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="12">
         <v>20</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="12">
         <v>1</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="C28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="16">
+        <v>20</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="22">
-        <v>20</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="22">
-        <v>0</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
@@ -1537,6 +1532,11 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some tweaks. Clarified super stats in leveling doc
</commit_message>
<xml_diff>
--- a/SupersNew/characters/Beetle.xlsx
+++ b/SupersNew/characters/Beetle.xlsx
@@ -1890,6 +1890,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="B2:F2"/>
@@ -1897,11 +1902,6 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" orientation="landscape" r:id="rId1"/>

</xml_diff>